<commit_message>
updated req july 30
</commit_message>
<xml_diff>
--- a/reviews.xlsx
+++ b/reviews.xlsx
@@ -468,17 +468,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
+          <t>Adidas AF37 106055 Matte Black / Blue Eyeglasses AF37 10 6055 52mm</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Great item, great quality. Fast sender</t>
+          <t>The frames were exactly as described and I received them in a timely manner!! Would purchase from seller again!!!</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Buyer: c***d</t>
+          <t>Buyer: s***1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,17 +495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Carrera Champion Rubber Black / Gray Sunglasses BIL 62mm</t>
+          <t>Tom Ford 5516 055 Light Havana Gold / Blue Block Eyeglasses TF5516 055 48mm</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Item exactly as described, fast shipping A+</t>
+          <t>Awesome. Thank y</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Buyer: c***7</t>
+          <t>Buyer: o***b</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -522,17 +522,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
+          <t>Tom Ford 5873 005 Shiny Black Tortoise / Blue Block Eyeglasses TF5873-B 005 49mm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Very nice item and the shipping was very quick.  I would definitely recommend this seller and I would not hesitate to deal with again in the future.</t>
+          <t>Thanks for a great pair of glasses. Quick shipping!!!</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Buyer: 6***t</t>
+          <t>Buyer: 7***1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -549,17 +549,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tom Ford 5587-B 053 Tortoise / Blue Block Eyeglasses TF5587 053 53mm</t>
+          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Really good communication with seller, very helpful, despatched quickly, item exactly as described. Recommended</t>
+          <t>Great item, great quality. Fast sender</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buyer: v***d</t>
+          <t>Buyer: c***d</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -576,17 +576,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ZERORH+ TITANO Silver Gray Titanium Eyeglasses RH195-01 55mm</t>
+          <t>Carrera Champion Rubber Black / Gray Sunglasses BIL 62mm</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Love them!</t>
+          <t>Item exactly as described, fast shipping A+</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buyer: 1***o</t>
+          <t>Buyer: c***7</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -603,17 +603,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tom Ford 5313 001 Shiny Black Eyeglasses TF5313 001 55mm</t>
+          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Super service and super glasses! Thank you</t>
+          <t>Very nice item and the shipping was very quick.  I would definitely recommend this seller and I would not hesitate to deal with again in the future.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Buyer: o***k</t>
+          <t>Buyer: 6***t</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -630,17 +630,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tag Heuer 501 004 Tortoise Brown Eyeglasses TH501-004 Spring Hinges 57mm</t>
+          <t>Tom Ford 5587-B 053 Tortoise / Blue Block Eyeglasses TF5587 053 53mm</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Item as pictured and described</t>
+          <t>Really good communication with seller, very helpful, despatched quickly, item exactly as described. Recommended</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Buyer: u***s</t>
+          <t>Buyer: v***d</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -657,17 +657,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Barton Perreira HEIST Pewter Matte Black / Blue Gradient Sunglasses MDT PEW STB</t>
+          <t>ZERORH+ TITANO Silver Gray Titanium Eyeglasses RH195-01 55mm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Item arrived promptly and as described</t>
+          <t>Love them!</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Buyer: 0***7</t>
+          <t>Buyer: 1***o</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -684,17 +684,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tom Ford 5590-B 052 Havana Ruthenium / Blue Block Eyeglasses TF5590 052 50mm</t>
+          <t>Tom Ford 5313 001 Shiny Black Eyeglasses TF5313 001 55mm</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Highly recommended</t>
+          <t>Super service and super glasses! Thank you</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Buyer: c***f</t>
+          <t>Buyer: o***k</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -711,22 +711,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6055 INVOKE Iron / Dark Gray Eyeglasses AF20 006055 54mm</t>
+          <t>Tag Heuer 501 004 Tortoise Brown Eyeglasses TH501-004 Spring Hinges 57mm</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bought these to replace another set of frames (same model) that I've had for many years. They're very comfortable, and I'm relieved to have found an identical replacement. Item arrived several weeks before the estimated delivery date. Thanks!</t>
+          <t>Item as pictured and described</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Buyer: 5***a</t>
+          <t>Buyer: u***s</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Past month</t>
+          <t>Past 6 months</t>
         </is>
       </c>
     </row>
@@ -738,17 +738,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tag Heuer AUTOMATIC 883 203 Chocolate / Brown Outdoors Sunglasses TH0883 203</t>
+          <t>Barton Perreira HEIST Pewter Matte Black / Blue Gradient Sunglasses MDT PEW STB</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Thank you!</t>
+          <t>Item arrived promptly and as described</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Buyer: t***7</t>
+          <t>Buyer: 0***7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -765,17 +765,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
+          <t>Tom Ford 5590-B 052 Havana Ruthenium / Blue Block Eyeglasses TF5590 052 50mm</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Excellent quality, good price and fast shipping</t>
+          <t>Highly recommended</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Buyer: 0***e</t>
+          <t>Buyer: c***f</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -792,17 +792,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tom Ford 5474 32E Gold Eyeglasses + Brown Clip TF5474-32E 53mm</t>
+          <t>Adidas AF20 00 6055 INVOKE Iron / Dark Gray Eyeglasses AF20 006055 54mm</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Top class, thanks</t>
+          <t>Bought these to replace another set of frames (same model) that I've had for many years. They're very comfortable, and I'm relieved to have found an identical replacement. Item arrived several weeks before the estimated delivery date. Thanks!</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Buyer: s***s</t>
+          <t>Buyer: 5***a</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -819,17 +819,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6057 INVOKE Amazon Red / Black Eyeglasses AF20 006057 54mm</t>
+          <t>Tag Heuer AUTOMATIC 883 203 Chocolate / Brown Outdoors Sunglasses TH0883 203</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Aritkel kam wie beschrieben und sehr gut verpackt an.</t>
+          <t>Thank you!</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Buyer: e***e</t>
+          <t>Buyer: t***7</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -846,17 +846,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tag Heuer 3052 003 Reflex Gray Eyeglasses TH3052-003 47mm</t>
+          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Thank you very much</t>
+          <t>Excellent quality, good price and fast shipping</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Buyer: i***i</t>
+          <t>Buyer: 0***e</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -873,17 +873,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tom Ford 5489 052 Havana Eyeglasses TF5489 052 48mm</t>
+          <t>Tom Ford 5474 32E Gold Eyeglasses + Brown Clip TF5474-32E 53mm</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Thank you so much for getting me these frames in such a timely fashion. Your process from start to finish was outstanding and I love my new frames again thanks for a positive experience!!!</t>
+          <t>Top class, thanks</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Buyer: 4***t</t>
+          <t>Buyer: s***s</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -900,17 +900,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MONCLER MC014-V03 Green Gunmetal Titanium Eyeglasses MC 014-V03 52mm</t>
+          <t>Adidas AF20 00 6057 INVOKE Amazon Red / Black Eyeglasses AF20 006057 54mm</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>I positively love these frames!! Just wish they came with original case.</t>
+          <t>Aritkel kam wie beschrieben und sehr gut verpackt an.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Buyer: a***n</t>
+          <t>Buyer: e***e</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -927,17 +927,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Just Cavalli 323S 14B Blue Silver / Grey Sunglasses JC323 14B 58mm</t>
+          <t>Tag Heuer 3052 003 Reflex Gray Eyeglasses TH3052-003 47mm</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>It was great experience and product, bought it for my husband and he loved them</t>
+          <t>Thank you very much</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Buyer: o***o</t>
+          <t>Buyer: i***i</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -954,17 +954,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Just Cavalli 323S 14B Blue Silver / Grey Sunglasses JC323 14B 58mm</t>
+          <t>Tom Ford 5489 052 Havana Eyeglasses TF5489 052 48mm</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Fast shipping...thank you.</t>
+          <t>Thank you so much for getting me these frames in such a timely fashion. Your process from start to finish was outstanding and I love my new frames again thanks for a positive experience!!!</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Buyer: a***a</t>
+          <t>Buyer: 4***t</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -981,17 +981,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lacoste Eyeglasses Sunglasses Medium Green Hard Case With Cloth</t>
+          <t>MONCLER MC014-V03 Green Gunmetal Titanium Eyeglasses MC 014-V03 52mm</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Very Fast shipping, good comunnication, great communication A++++</t>
+          <t>I positively love these frames!! Just wish they came with original case.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Buyer: o***d</t>
+          <t>Buyer: a***n</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1008,17 +1008,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tom Ford 5873 001 Shiny Black / Blue Block Eyeglasses TF5873-B 001 49mm</t>
+          <t>Just Cavalli 323S 14B Blue Silver / Grey Sunglasses JC323 14B 58mm</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>As promised and on time! 5 stars</t>
+          <t>It was great experience and product, bought it for my husband and he loved them</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Buyer: t***_</t>
+          <t>Buyer: o***o</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1035,17 +1035,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tom Ford 5408 052 Dark Havana Eyeglasses TF5408 052 56mm</t>
+          <t>Just Cavalli 323S 14B Blue Silver / Grey Sunglasses JC323 14B 58mm</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Great quality product!</t>
+          <t>Fast shipping...thank you.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Buyer: e***e</t>
+          <t>Buyer: a***a</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1062,17 +1062,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Tom Ford 5873 001 Shiny Black / Blue Block Eyeglasses TF5873-B 001 49mm</t>
+          <t>Lacoste Eyeglasses Sunglasses Medium Green Hard Case With Cloth</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>On time and as promised</t>
+          <t>Very Fast shipping, good comunnication, great communication A++++</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Buyer: t***_</t>
+          <t>Buyer: o***d</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1089,17 +1089,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
+          <t>Tom Ford 5873 001 Shiny Black / Blue Block Eyeglasses TF5873-B 001 49mm</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Excellent item, low price, and extremely fast shipping</t>
+          <t>As promised and on time! 5 stars</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Buyer: 0***e</t>
+          <t>Buyer: t***_</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1116,17 +1116,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MONTBLANC MB0723 001 Shiny Black Eyeglasses MB 723 001 55mm</t>
+          <t>Tom Ford 5408 052 Dark Havana Eyeglasses TF5408 052 56mm</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>as described, would do business with again, AAA+++</t>
+          <t>Great quality product!</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Buyer: r***r</t>
+          <t>Buyer: e***e</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1143,17 +1143,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tom Ford IVANNA 372 53W Havana / Blue Gradient Sunglasses TF372 53W 64mm</t>
+          <t>Tom Ford 5873 001 Shiny Black / Blue Block Eyeglasses TF5873-B 001 49mm</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Pretty</t>
+          <t>On time and as promised</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Buyer: 1***r</t>
+          <t>Buyer: t***_</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1170,17 +1170,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Tom Ford NIKA 523 52F Dark Havana / Purple Gradient Sunglasses TF523 52F 56mm</t>
+          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Absolutely beautiful. Came with a little cleaning kit. I will buy from here again. 🫶🏼</t>
+          <t>Excellent item, low price, and extremely fast shipping</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Buyer: g***i</t>
+          <t>Buyer: 0***e</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1197,17 +1197,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Tom Ford 5207 083 Havana Eyeglasses TF5207 083 49mm</t>
+          <t>MONTBLANC MB0723 001 Shiny Black Eyeglasses MB 723 001 55mm</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Professional. Quick and exactly as described.</t>
+          <t>as described, would do business with again, AAA+++</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Buyer: d***r</t>
+          <t>Buyer: r***r</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1224,17 +1224,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ZERORH+ FORMULA Brown &amp; Blue Eyeglasses RH222 222-05 53mm</t>
+          <t>Tom Ford IVANNA 372 53W Havana / Blue Gradient Sunglasses TF372 53W 64mm</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>Pretty</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Buyer: t***c</t>
+          <t>Buyer: 1***r</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1251,17 +1251,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ZERORH+ FORMULA Eyeglasses RH217</t>
+          <t>Tom Ford NIKA 523 52F Dark Havana / Purple Gradient Sunglasses TF523 52F 56mm</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>good!</t>
+          <t>Absolutely beautiful. Came with a little cleaning kit. I will buy from here again. 🫶🏼</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Buyer: t***c</t>
+          <t>Buyer: g***i</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1278,17 +1278,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tag Heuer 7603-002 Track Brown Havana Orange Eyeglasses TH7603 002 50mm</t>
+          <t>Tom Ford 5207 083 Havana Eyeglasses TF5207 083 49mm</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Great seller. Fast shipping. Thank you.</t>
+          <t>Professional. Quick and exactly as described.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Buyer: i***r</t>
+          <t>Buyer: d***r</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1305,17 +1305,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tom Ford 5415 054 Tortoise Eyeglasses TF5415 054 50mm</t>
+          <t>ZERORH+ FORMULA Brown &amp; Blue Eyeglasses RH222 222-05 53mm</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Great Price, easy transaction and great experience. SunRayCity also included accessories I didn't expect. Nice touch!</t>
+          <t>good</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Buyer: u***r</t>
+          <t>Buyer: t***c</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1332,17 +1332,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Tag Heuer 7604 003 Track Navy Blue Gray Eyeglasses 7604-003 56mm</t>
+          <t>ZERORH+ FORMULA Eyeglasses RH217</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Love these frames!</t>
+          <t>good!</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Buyer: n***r</t>
+          <t>Buyer: t***c</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1359,99 +1359,99 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Tag Heuer 7603-002 Track Brown Havana Orange Eyeglasses TH7603 002 50mm</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Great seller. Fast shipping. Thank you.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Buyer: i***r</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Past 6 months</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Tom Ford 5415 054 Tortoise Eyeglasses TF5415 054 50mm</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Great Price, easy transaction and great experience. SunRayCity also included accessories I didn't expect. Nice touch!</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Buyer: u***r</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Past 6 months</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Tag Heuer 7604 003 Track Navy Blue Gray Eyeglasses 7604-003 56mm</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Love these frames!</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Buyer: n***r</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Past 6 months</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>Rayban Aviator 3025 L0205 Gold / G-15 Sunglasses Made in Italy 58mm</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>The seller is A+++++++.
 Thank you very much.</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Buyer: f***e</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Past 6 months</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Tom Ford 5421 074 Rose Pink Eyeglasses TF5421 074 53mm</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Excellent brand new frames.Fast delivery, perfect transaction. Thanks</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Buyer: e***1</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Past 6 months</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Serengeti Martino Dark Tortoise / Green Polarized Sunglasses 7528</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>+++TOP+++</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Buyer: e***d</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Past 6 months</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Tom Ford 5007 Q41 Marble Brown Eyeglasses TF5007 Q41 51mm</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Great</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Buyer: a***a</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1468,17 +1468,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Tom Ford 5424 001 Black Eyeglasses TF5424 001 55mm</t>
+          <t>Tom Ford 5421 074 Rose Pink Eyeglasses TF5421 074 53mm</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Flawless transaction!  Was not sure about the size but better than expected!!</t>
+          <t>Excellent brand new frames.Fast delivery, perfect transaction. Thanks</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Buyer: z***e</t>
+          <t>Buyer: e***1</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1495,17 +1495,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Tom Ford 5762 052 Dark Havana / Blue Block Eyeglasses TF5762-B 052 55mm</t>
+          <t>Serengeti Martino Dark Tortoise / Green Polarized Sunglasses 7528</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Exactly as described, brand new with no defects, came with certificate of authenticity. Lightning fast shipping and delivery plus seller included some extras, such as cleaner and microfibre cloth which is highly appreciated. Would definitely recommend. Wonderful experience, A+++ Thank you !!!</t>
+          <t>+++TOP+++</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Buyer: z***o</t>
+          <t>Buyer: e***d</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1522,17 +1522,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
+          <t>Tom Ford 5007 Q41 Marble Brown Eyeglasses TF5007 Q41 51mm</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Great seller.</t>
+          <t>Great</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Buyer: -***x</t>
+          <t>Buyer: a***a</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1549,17 +1549,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Adidas AF23 50 6057 INVOKE Black / Night Flash Eyeglasses AF23 506057 53mm</t>
+          <t>Tom Ford 5424 001 Black Eyeglasses TF5424 001 55mm</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Fantastic seller! They ship very quickly and will negotiate if you use the offer button. They are very fair and with the item they include some extras, which is appreciated. Next time I’m looking for frames at an excellent price, I will shop here. Many thanks.</t>
+          <t>Flawless transaction!  Was not sure about the size but better than expected!!</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Buyer: t***c</t>
+          <t>Buyer: z***e</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1576,17 +1576,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Adidas AF39 00 6050 CONVERTOR Black Eyeglasses AF39 006050 57mm Adaptable Temple</t>
+          <t>Tom Ford 5762 052 Dark Havana / Blue Block Eyeglasses TF5762-B 052 55mm</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Exactly what was advertised, with extras I appreciated but didn't expect, such as cleaner and extra microfiber cloths. Would buy from this seller again!</t>
+          <t>Exactly as described, brand new with no defects, came with certificate of authenticity. Lightning fast shipping and delivery plus seller included some extras, such as cleaner and microfibre cloth which is highly appreciated. Would definitely recommend. Wonderful experience, A+++ Thank you !!!</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Buyer: 8***7</t>
+          <t>Buyer: z***o</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1603,17 +1603,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Carrera 5011 Camouflage Pink / Pink Sunglasses 5011/S 8GW 54mm</t>
+          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Happy with the glasses. Prompt delivery.</t>
+          <t>Great seller.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Buyer: i***6</t>
+          <t>Buyer: -***x</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1630,17 +1630,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Tom Ford 5375 056 Dark Havana Eyeglasses TF5375 056 Asian Fit 55mm</t>
+          <t>Adidas AF23 50 6057 INVOKE Black / Night Flash Eyeglasses AF23 506057 53mm</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Items arrived as listed. I'll purchase from the seller again.</t>
+          <t>Fantastic seller! They ship very quickly and will negotiate if you use the offer button. They are very fair and with the item they include some extras, which is appreciated. Next time I’m looking for frames at an excellent price, I will shop here. Many thanks.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Buyer: _***_</t>
+          <t>Buyer: t***c</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1657,17 +1657,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tom Ford 5207 005 Dark Brown Eyeglasses TF5207 005 49mm</t>
+          <t>Adidas AF39 00 6050 CONVERTOR Black Eyeglasses AF39 006050 57mm Adaptable Temple</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Thanks!  As described. A+</t>
+          <t>Exactly what was advertised, with extras I appreciated but didn't expect, such as cleaner and extra microfiber cloths. Would buy from this seller again!</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Buyer: s***t</t>
+          <t>Buyer: 8***7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1679,22 +1679,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Negative feedback rating</t>
+          <t>Positive feedback rating</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>PROSHADE Sun Visor Lanyard 3 In 1 Eyewear Case</t>
+          <t>Carrera 5011 Camouflage Pink / Pink Sunglasses 5011/S 8GW 54mm</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Nothing against the seller, item was as described but it doesn’t work. Visor does not stay up and straight.</t>
+          <t>Happy with the glasses. Prompt delivery.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Buyer: y***o</t>
+          <t>Buyer: i***6</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1711,17 +1711,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tom Ford 5172 028 Gold Round Eyeglasses TF5172 028 40mm SMALL</t>
+          <t>Tom Ford 5375 056 Dark Havana Eyeglasses TF5375 056 Asian Fit 55mm</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Qualitative good product as described</t>
+          <t>Items arrived as listed. I'll purchase from the seller again.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Buyer: n***i</t>
+          <t>Buyer: _***_</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1738,17 +1738,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Tom Ford 5455 056 Havana Amber Oval Eyeglasses TF5455 056 50mm</t>
+          <t>Tom Ford 5207 005 Dark Brown Eyeglasses TF5207 005 49mm</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Thanks I love them . I hand them and they were hard to find. 💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿</t>
+          <t>Thanks!  As described. A+</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Buyer: u***5</t>
+          <t>Buyer: s***t</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1760,22 +1760,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Positive feedback rating</t>
+          <t>Negative feedback rating</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Tag Heuer 8007 003 Trends Chocolate Havane Black Eyeglasses 8007-003 56mm</t>
+          <t>PROSHADE Sun Visor Lanyard 3 In 1 Eyewear Case</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Quick, highly recommended seller! Thanks!</t>
+          <t>Nothing against the seller, item was as described but it doesn’t work. Visor does not stay up and straight.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Buyer: 2***2</t>
+          <t>Buyer: y***o</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1792,17 +1792,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Tom Ford 5291 052 Brown Turquoise Eyeglasses TF5291 052 55mm</t>
+          <t>Tom Ford 5172 028 Gold Round Eyeglasses TF5172 028 40mm SMALL</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nice glasses, fast shipping great seller</t>
+          <t>Qualitative good product as described</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Buyer: b***b</t>
+          <t>Buyer: n***i</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1819,17 +1819,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Tom Ford 5304 093 Gray Stripe Eyeglasses TF5304 093 54mm</t>
+          <t>Tom Ford 5455 056 Havana Amber Oval Eyeglasses TF5455 056 50mm</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Excellent! Thanks!!!</t>
+          <t>Thanks I love them . I hand them and they were hard to find. 💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿💪🏿</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Buyer: p***o</t>
+          <t>Buyer: u***5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1846,17 +1846,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260 64mm</t>
+          <t>Tag Heuer 8007 003 Trends Chocolate Havane Black Eyeglasses 8007-003 56mm</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Thank you</t>
+          <t>Quick, highly recommended seller! Thanks!</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Buyer: e***e</t>
+          <t>Buyer: 2***2</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1873,17 +1873,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
+          <t>Tom Ford 5291 052 Brown Turquoise Eyeglasses TF5291 052 55mm</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Terrific Seller</t>
+          <t>Nice glasses, fast shipping great seller</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Buyer: t***3</t>
+          <t>Buyer: b***b</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1900,17 +1900,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SPY CALIBER Soft Matte Black / Happy Gray Green Sunglasses 673374973863 59mm</t>
+          <t>Tom Ford 5304 093 Gray Stripe Eyeglasses TF5304 093 54mm</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Perfect!  Crazy fast shipping too.  A+++</t>
+          <t>Excellent! Thanks!!!</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Buyer: i***h</t>
+          <t>Buyer: p***o</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1927,17 +1927,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Tom Ford CLINT Havana / Yellow Sunglasses TF537 48E 52mm</t>
+          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260 64mm</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Everything was perfect.</t>
+          <t>Thank you</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Buyer: o***n</t>
+          <t>Buyer: e***e</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1954,17 +1954,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tom Ford 5313 055 Dark Havana Eyeglasses TF5313 055 55mm</t>
+          <t>Serengeti Ramone Satin Bronze / Cool Photo Gray Polarmax Sunglasses 7157</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Thank you very much.</t>
+          <t>Terrific Seller</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Buyer: o***i</t>
+          <t>Buyer: t***3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1981,17 +1981,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Tom Ford CLINT Havana / Yellow Sunglasses TF537 48E 52mm</t>
+          <t>SPY CALIBER Soft Matte Black / Happy Gray Green Sunglasses 673374973863 59mm</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Perfect thank you</t>
+          <t>Perfect!  Crazy fast shipping too.  A+++</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Buyer: a***l</t>
+          <t>Buyer: i***h</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2008,17 +2008,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Tom Ford 5163 55A Havana Eyeglasses TF5163 55A 53mm</t>
+          <t>Tom Ford CLINT Havana / Yellow Sunglasses TF537 48E 52mm</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Exactly as described.</t>
+          <t>Everything was perfect.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Buyer: 4***4</t>
+          <t>Buyer: o***n</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2035,17 +2035,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Adidas A628 50 6054 Black Eyeglasses 628 506054 55mm</t>
+          <t>Tom Ford 5313 055 Dark Havana Eyeglasses TF5313 055 55mm</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Seller helped me verify that these will work with my existing lenses. I'm a repeat customer and have had excellent results with SunRayCity!</t>
+          <t>Thank you very much.</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Buyer: m***i</t>
+          <t>Buyer: o***i</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2062,17 +2062,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Tom Ford 5590-B 055 Havana Titanium Gold / Blue Block Eyeglasses TF5590 055 50mm</t>
+          <t>Tom Ford CLINT Havana / Yellow Sunglasses TF537 48E 52mm</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Thanks for a great product!</t>
+          <t>Perfect thank you</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Buyer: 8***g</t>
+          <t>Buyer: a***l</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2089,17 +2089,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Tom Ford 5483 028 Shiny Rose Gold Titanium Eyeglasses TF5483 028 52mm</t>
+          <t>Tom Ford 5163 55A Havana Eyeglasses TF5163 55A 53mm</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>Exactly as described.</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Buyer: u***9</t>
+          <t>Buyer: 4***4</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2116,17 +2116,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
+          <t>Adidas A628 50 6054 Black Eyeglasses 628 506054 55mm</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Excellent seller. Great products. Fast delivery and also received some extra bonuses which was a delightful surprise. Highly recommended and will purchase more.  A+++++</t>
+          <t>Seller helped me verify that these will work with my existing lenses. I'm a repeat customer and have had excellent results with SunRayCity!</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Buyer: o***i</t>
+          <t>Buyer: m***i</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2143,17 +2143,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Adidas AF23 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF23 406053 55mm</t>
+          <t>Tom Ford 5590-B 055 Havana Titanium Gold / Blue Block Eyeglasses TF5590 055 50mm</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Seller has agreed to send the item again........when it arrives I will be happy!</t>
+          <t>Thanks for a great product!</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Buyer: s***e</t>
+          <t>Buyer: 8***g</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2170,17 +2170,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Giorgio Armani 456 PRP X7 Brown / Brown Sunglasses 60mm</t>
+          <t>Tom Ford 5483 028 Shiny Rose Gold Titanium Eyeglasses TF5483 028 52mm</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Great seller fast delivery very pleased￼A+++++</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Buyer: a***a</t>
+          <t>Buyer: u***9</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2197,12 +2197,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Tom Ford 5549-B 002 Black / Blue Block Eyeglasses TF5549 002 52mm</t>
+          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Great</t>
+          <t>Excellent seller. Great products. Fast delivery and also received some extra bonuses which was a delightful surprise. Highly recommended and will purchase more.  A+++++</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2224,17 +2224,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Tom Ford 5504 052 Dark Havana Gold Eyeglasses TF5504 052 54mm</t>
+          <t>Adidas AF23 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF23 406053 55mm</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Fast shipping, Accurate item,  Great seller. I would definitely do business with again.</t>
+          <t>Seller has agreed to send the item again........when it arrives I will be happy!</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Buyer: l***_</t>
+          <t>Buyer: s***e</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2251,17 +2251,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Tom Ford 5549-B 002 Black / Blue Block Eyeglasses TF5549 002 52mm</t>
+          <t>Giorgio Armani 456 PRP X7 Brown / Brown Sunglasses 60mm</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Got here ahead of time and was exactly as ordered</t>
+          <t>Great seller fast delivery very pleased￼A+++++</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Buyer: j***6</t>
+          <t>Buyer: a***a</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2278,17 +2278,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Tom Ford 5163 55A Havana Eyeglasses TF5163 55A 53mm</t>
+          <t>Tom Ford 5549-B 002 Black / Blue Block Eyeglasses TF5549 002 52mm</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Alles bestens! Gerne wieder. Vielen Dank!</t>
+          <t>Great</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Buyer: o***o</t>
+          <t>Buyer: o***i</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2305,17 +2305,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Tom Ford CHRISTOPHER 02 Shiny Black / Gray Sunglasses TF633 001 0633 49mm</t>
+          <t>Tom Ford 5504 052 Dark Havana Gold Eyeglasses TF5504 052 54mm</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Amazing seller . Flawless transaction</t>
+          <t>Fast shipping, Accurate item,  Great seller. I would definitely do business with again.</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Buyer: j***l</t>
+          <t>Buyer: l***_</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2332,17 +2332,17 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
+          <t>Tom Ford 5549-B 002 Black / Blue Block Eyeglasses TF5549 002 52mm</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Quick delivery. Item was nicely packed. Recommended ebayer. A+++++++++ Thanks!</t>
+          <t>Got here ahead of time and was exactly as ordered</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Buyer: l***0</t>
+          <t>Buyer: j***6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2359,17 +2359,17 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>MONCLER MC512-V04 Striped Gray Eyeglasses MC 512-V04</t>
+          <t>Tom Ford 5163 55A Havana Eyeglasses TF5163 55A 53mm</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>THANK YOU... A+ SELLER.....</t>
+          <t>Alles bestens! Gerne wieder. Vielen Dank!</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Buyer: o***2</t>
+          <t>Buyer: o***o</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2386,17 +2386,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Tag Heuer 821 009 Automatic Gray Orange Eyeglasses 0821-009 56mm</t>
+          <t>Tom Ford CHRISTOPHER 02 Shiny Black / Gray Sunglasses TF633 001 0633 49mm</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Really smooth transaction, speedy delivery too, can highly recommend.....</t>
+          <t>Amazing seller . Flawless transaction</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Buyer: m***2</t>
+          <t>Buyer: j***l</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2413,17 +2413,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Moncler MC507-01 Tortoise / Gray Pelvoux Sunglasses MC 507-01 58mm</t>
+          <t>Carrera Sunglasses Small Black Leather Hard Case With Cloth</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Received faster than expected. Very good quality, with certificate of authentication. I had this for over 10 years and lost them in the water this year. Really happy to have been able to get them again!</t>
+          <t>Quick delivery. Item was nicely packed. Recommended ebayer. A+++++++++ Thanks!</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Buyer: d***8</t>
+          <t>Buyer: l***0</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2440,17 +2440,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Tom Ford 5514 083 Violet Eyeglasses TF5514 083 54mm</t>
+          <t>MONCLER MC512-V04 Striped Gray Eyeglasses MC 512-V04</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Great seller with fantastic communication. Fast Shipping and Perfect Condition. Thank you!</t>
+          <t>THANK YOU... A+ SELLER.....</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Buyer: s***i</t>
+          <t>Buyer: o***2</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2467,17 +2467,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6052 INVOKE Shiny Brown / Orange Eyeglasses AF20 006052 56mm</t>
+          <t>Tag Heuer 821 009 Automatic Gray Orange Eyeglasses 0821-009 56mm</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Perfect.</t>
+          <t>Really smooth transaction, speedy delivery too, can highly recommend.....</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Buyer: n***g</t>
+          <t>Buyer: m***2</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2494,17 +2494,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Tom Ford 5586-B 001 Black Blue Block Eyeglasses TF5586 001 56mm</t>
+          <t>Moncler MC507-01 Tortoise / Gray Pelvoux Sunglasses MC 507-01 58mm</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>A+++</t>
+          <t>Received faster than expected. Very good quality, with certificate of authentication. I had this for over 10 years and lost them in the water this year. Really happy to have been able to get them again!</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Buyer: y***7</t>
+          <t>Buyer: d***8</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2521,17 +2521,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Adidas AF23 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF23 406053 55mm</t>
+          <t>Tom Ford 5514 083 Violet Eyeglasses TF5514 083 54mm</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Great item, exactly as described and fast international shipping. Thanks</t>
+          <t>Great seller with fantastic communication. Fast Shipping and Perfect Condition. Thank you!</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Buyer: u***o</t>
+          <t>Buyer: s***i</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2548,22 +2548,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Carrera 7015 Xcede Matte Black / Gray Polarized Sunglasses 7015/S 03P 61mm</t>
+          <t>Adidas AF20 00 6052 INVOKE Shiny Brown / Orange Eyeglasses AF20 006052 56mm</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Outstanding transaction! Super fast responses and shipping! These sunglasses are PERFECT! Thanks for the great service and fast shipping! Awesome seller!</t>
+          <t>Perfect.</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Buyer: k***v</t>
+          <t>Buyer: n***g</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Past year</t>
+          <t>More than a year ago</t>
         </is>
       </c>
     </row>
@@ -2575,17 +2575,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6055 INVOKE Iron / Dark Gray Eyeglasses AF20 006055 54mm</t>
+          <t>Tom Ford 5586-B 001 Black Blue Block Eyeglasses TF5586 001 56mm</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Love these frames as they are so comfortable.</t>
+          <t>A+++</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Buyer: 6***m</t>
+          <t>Buyer: y***7</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2602,17 +2602,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>GUCCI GG0060O 004 Flowers Multicolor Eyeglasses GG 600 49mm</t>
+          <t>Adidas AF23 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF23 406053 55mm</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Thank you SunRayCity!  I love this frame, and you helped me replace the same ones that I lost! I appreciate your sending this so quickly and the other little goodies you includes. I’m so happy!</t>
+          <t>Great item, exactly as described and fast international shipping. Thanks</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Buyer: o***e</t>
+          <t>Buyer: u***o</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2629,17 +2629,17 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Tom Ford 5291 005 Black Turquoise Eyeglasses TF5291 005 55mm</t>
+          <t>Carrera 7015 Xcede Matte Black / Gray Polarized Sunglasses 7015/S 03P 61mm</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>A+++++</t>
+          <t>Outstanding transaction! Super fast responses and shipping! These sunglasses are PERFECT! Thanks for the great service and fast shipping! Awesome seller!</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Buyer: l***e</t>
+          <t>Buyer: k***v</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2656,17 +2656,17 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Tom Ford Ekaterina 363 71Z Bordeaux / Purple Gradient Sunglasses TF363 71Z 150mm</t>
+          <t>Adidas AF20 00 6055 INVOKE Iron / Dark Gray Eyeglasses AF20 006055 54mm</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Item in perfect condition and arrived promptly.</t>
+          <t>Love these frames as they are so comfortable.</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Buyer: n***k</t>
+          <t>Buyer: 6***m</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2683,99 +2683,99 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
+          <t>GUCCI GG0060O 004 Flowers Multicolor Eyeglasses GG 600 49mm</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Thank you SunRayCity!  I love this frame, and you helped me replace the same ones that I lost! I appreciate your sending this so quickly and the other little goodies you includes. I’m so happy!</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Buyer: o***e</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Tom Ford 5291 005 Black Turquoise Eyeglasses TF5291 005 55mm</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>A+++++</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Buyer: l***e</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Tom Ford Ekaterina 363 71Z Bordeaux / Purple Gradient Sunglasses TF363 71Z 150mm</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Item in perfect condition and arrived promptly.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Buyer: n***k</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
           <t>Tom Ford 5226 083 Purple Tortoise Eyeglasses TF5226 083 54mm</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>The seller was right on about the product 
 Everyone likes the eye frame on me I’m not to share yet once I see my eye doctor in fall I get my new lenses in I’m not saying I don’t like them their different from other eyeglass frames that’s for sure</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>Buyer: r***m</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Tom Ford NINA 373 01B Black Gold / Gray Gradient Sunglasses TF373 01B 56mm</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Love these sunglasses! My favorite Tom Ford style ever. They arrived sooner than expected and well packaged. Although a vintage style, these are new. I was delighted to find them on eBay!</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Buyer: h***2</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Tag Heuer 825 009 Gray Orange Eyeglasses TH825-009 57mm</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>BUENAS TARDES. EL PEDIDO HA LLEGADO HOY 03/07/2023.LAS GAFAS VIENEN EMBALADAS PERFECTAMENTE Y A LA ENTREGA HE PAGADO LOS ARANCELES CORRESPONDIENTES,EN ÉSTE CASO HAN SIDO 38,38€. LAS GAFAS SON EXACTAMENTE EL MODELO QUE HABÍA ELEGIDO.VENDEDOR EXCELENTE.</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Buyer: b***-</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Tom Ford 5424 056A Light Havana Purple Eyeglasses TF5424 056A 53mm</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>great vendor. Frames exactly as described , brand new with case cleaning cloth and sunglass cover. Excellent--will purchase again from vendor</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Buyer: 2***m</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2792,17 +2792,17 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>MONTBLANC MB0674 013 Satin Ruthenium Eyeglasses MB 674 013 56mm</t>
+          <t>Tom Ford NINA 373 01B Black Gold / Gray Gradient Sunglasses TF373 01B 56mm</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>All good, great price and delivered as advertised</t>
+          <t>Love these sunglasses! My favorite Tom Ford style ever. They arrived sooner than expected and well packaged. Although a vintage style, these are new. I was delighted to find them on eBay!</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Buyer: i***i</t>
+          <t>Buyer: h***2</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2819,17 +2819,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Barton Perreira SAMUEL Black Eyeglasses BLA 50mm</t>
+          <t>Tag Heuer 825 009 Gray Orange Eyeglasses TH825-009 57mm</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Love my glasses they were as expected fast shipping too!</t>
+          <t>BUENAS TARDES. EL PEDIDO HA LLEGADO HOY 03/07/2023.LAS GAFAS VIENEN EMBALADAS PERFECTAMENTE Y A LA ENTREGA HE PAGADO LOS ARANCELES CORRESPONDIENTES,EN ÉSTE CASO HAN SIDO 38,38€. LAS GAFAS SON EXACTAMENTE EL MODELO QUE HABÍA ELEGIDO.VENDEDOR EXCELENTE.</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Buyer: a***-</t>
+          <t>Buyer: b***-</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2846,17 +2846,17 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Adidas AF23 50 6054 INVOKE Black /Gray Eyeglasses AF23 506054 53mm</t>
+          <t>Tom Ford 5424 056A Light Havana Purple Eyeglasses TF5424 056A 53mm</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>An excellent seller! The item shipped out quickly and came with a tracking number.  Shipping was very fast and secure. Am very pleased with my item.</t>
+          <t>great vendor. Frames exactly as described , brand new with case cleaning cloth and sunglass cover. Excellent--will purchase again from vendor</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Buyer: t***c</t>
+          <t>Buyer: 2***m</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2873,17 +2873,17 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Tom Ford Snowdon Beige / Gray Gradient Sunglasses TF237 60B 50mm</t>
+          <t>MONTBLANC MB0674 013 Satin Ruthenium Eyeglasses MB 674 013 56mm</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>A++++++++++++++++</t>
+          <t>All good, great price and delivered as advertised</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Buyer: 5***5</t>
+          <t>Buyer: i***i</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2900,17 +2900,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Bolle Draft Crystal Smoke / Photochromic Rose Gun Sunglasses 11470</t>
+          <t>Barton Perreira SAMUEL Black Eyeglasses BLA 50mm</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Great item great price fast shipping thank you</t>
+          <t>Love my glasses they were as expected fast shipping too!</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Buyer: d***e</t>
+          <t>Buyer: a***-</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2927,17 +2927,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Serengeti Martino Shiny Black / Sedona Polarized Sunglasses 7840</t>
+          <t>Adidas AF23 50 6054 INVOKE Black /Gray Eyeglasses AF23 506054 53mm</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Sunglasses were delivered as new.  Great shape.</t>
+          <t>An excellent seller! The item shipped out quickly and came with a tracking number.  Shipping was very fast and secure. Am very pleased with my item.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Buyer: 8***b</t>
+          <t>Buyer: t***c</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2954,17 +2954,17 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Barton Perreira HEIST Gold Tortoise / Gray Gradient Sunglasses EST ANG SMT</t>
+          <t>Tom Ford Snowdon Beige / Gray Gradient Sunglasses TF237 60B 50mm</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>FAST SHIPPING THANK YOU A+</t>
+          <t>A++++++++++++++++</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Buyer: e***n</t>
+          <t>Buyer: 5***5</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2981,17 +2981,17 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Serengeti Sangro Satin Black / Polarized Drivers Sunglasses 6998</t>
+          <t>Bolle Draft Crystal Smoke / Photochromic Rose Gun Sunglasses 11470</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>recommend this seller</t>
+          <t>Great item great price fast shipping thank you</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Buyer: i***n</t>
+          <t>Buyer: d***e</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3008,17 +3008,17 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Carrera 42 Horn Black / Gray Gradient Sunglasses 42/S 7J3</t>
+          <t>Serengeti Martino Shiny Black / Sedona Polarized Sunglasses 7840</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Gréât seller and auction. Thx</t>
+          <t>Sunglasses were delivered as new.  Great shape.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Buyer: 1***0</t>
+          <t>Buyer: 8***b</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3035,17 +3035,17 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>MONCLER MC010-S05 Gray / Gray Sunglasses MC 010-S05</t>
+          <t>Barton Perreira HEIST Gold Tortoise / Gray Gradient Sunglasses EST ANG SMT</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Thank you very fast</t>
+          <t>FAST SHIPPING THANK YOU A+</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Buyer: n***5</t>
+          <t>Buyer: e***n</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3062,17 +3062,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
+          <t>Serengeti Sangro Satin Black / Polarized Drivers Sunglasses 6998</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Fast shipping, great item, would definitely buy from again</t>
+          <t>recommend this seller</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Buyer: g***m</t>
+          <t>Buyer: i***n</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3089,17 +3089,17 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Tom Ford 5172 028 Gold Round Eyeglasses TF5172 028 40mm SMALL</t>
+          <t>Carrera 42 Horn Black / Gray Gradient Sunglasses 42/S 7J3</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Gréât seller and auction. Thx</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Buyer: h***w</t>
+          <t>Buyer: 1***0</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3116,17 +3116,17 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Tag Heuer 802 011 Automatic Matte Black White Eyeglasses 802-011</t>
+          <t>MONCLER MC010-S05 Gray / Gray Sunglasses MC 010-S05</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Thanks for the great transaction! Frames are awesome and shipping was fast. Highly recommended!!</t>
+          <t>Thank you very fast</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Buyer: h***a</t>
+          <t>Buyer: n***5</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3143,17 +3143,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Tom Ford 5460 045 Honey Eyeglasses TF5460 045 49mm</t>
+          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Good seller, no hassle.</t>
+          <t>Fast shipping, great item, would definitely buy from again</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Buyer: c***b</t>
+          <t>Buyer: g***m</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3170,17 +3170,17 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Adidas AF40 006054 CONVERTOR Matte Dark Brown / Orange Eyeglasses 55mm Adaptable</t>
+          <t>Tom Ford 5172 028 Gold Round Eyeglasses TF5172 028 40mm SMALL</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>very fast shipping</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Buyer: e***3</t>
+          <t>Buyer: h***w</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3197,99 +3197,99 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
+          <t>Tag Heuer 802 011 Automatic Matte Black White Eyeglasses 802-011</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Thanks for the great transaction! Frames are awesome and shipping was fast. Highly recommended!!</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Buyer: h***a</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Tom Ford 5460 045 Honey Eyeglasses TF5460 045 49mm</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Good seller, no hassle.</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Buyer: c***b</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Adidas AF40 006054 CONVERTOR Matte Dark Brown / Orange Eyeglasses 55mm Adaptable</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>very fast shipping</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Buyer: e***3</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
           <t>Tom Ford HAYES 934 01E Shiny Black / Brown Sunglasses TF934 01E 59mm</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>Great transaction, fast shipping - Thx!!
 A+</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
+      <c r="D106" t="inlineStr">
         <is>
           <t>Buyer: _***s</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Tag Heuer 3012 001 Reflex Black Gray Clear Eyeglasses TH3012 001 47mm</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>love these</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Buyer: e***i</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Tom Ford 5172 018 Silver Round Eyeglasses TF5172 018 40mm SMALL</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>As expected</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Buyer: t***t</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Brilliant service thank you</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Buyer: i***l</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -3306,17 +3306,17 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Adidas AF39 00 6050 CONVERTOR Black Eyeglasses AF39 006050 57mm Adaptable Temple</t>
+          <t>Tag Heuer 3012 001 Reflex Black Gray Clear Eyeglasses TH3012 001 47mm</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>the better adidas glasses frame, low weight, best fit</t>
+          <t>love these</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Buyer: v***8</t>
+          <t>Buyer: e***i</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3328,22 +3328,22 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Neutral feedback rating</t>
+          <t>Positive feedback rating</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Tom Ford 5365 024 Beige Eyeglasses TF5365 024 54mm</t>
+          <t>Tom Ford 5172 018 Silver Round Eyeglasses TF5172 018 40mm SMALL</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>I think these are seconds.  The coloring was inconsistent.  Either from firing or ? .</t>
+          <t>As expected</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Buyer: a***i</t>
+          <t>Buyer: t***t</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3360,17 +3360,17 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Tom Ford 5304 052 Dark Havana Eyeglasses TF5304 052 54mm</t>
+          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Was able to contact the seller. Since it s a global shipping I recommend at least putting the product in a plastic bag properly just in case or cover the lense cleaner cap with a tape. Glasses was in good condition and seller communication was prompt.</t>
+          <t>Brilliant service thank you</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Buyer: l***s</t>
+          <t>Buyer: i***l</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3387,99 +3387,99 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
+          <t>Adidas AF39 00 6050 CONVERTOR Black Eyeglasses AF39 006050 57mm Adaptable Temple</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>the better adidas glasses frame, low weight, best fit</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Buyer: v***8</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Neutral feedback rating</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Tom Ford 5365 024 Beige Eyeglasses TF5365 024 54mm</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>I think these are seconds.  The coloring was inconsistent.  Either from firing or ? .</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Buyer: a***i</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Tom Ford 5304 052 Dark Havana Eyeglasses TF5304 052 54mm</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Was able to contact the seller. Since it s a global shipping I recommend at least putting the product in a plastic bag properly just in case or cover the lense cleaner cap with a tape. Glasses was in good condition and seller communication was prompt.</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Buyer: l***s</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
           <t>Serengeti Milazzo Matte Black Polarized 555nm Sunglasses 6903</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>Got them grate sunglasses ever made.
 Best Regards</t>
         </is>
       </c>
-      <c r="D110" t="inlineStr">
+      <c r="D113" t="inlineStr">
         <is>
           <t>Buyer: 2***f</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Adidas A644 40 6052 Green Eyeglasses 644 406052 52mm</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>easy buy. great glasses and recieved some nice extras along with them. thank you very much. will purchase again.</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Buyer: o***g</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>MontBlanc Silver / Gray Sunglasses MB457S 16A</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Great product and fast shopping. Thank you! A+++++++</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Buyer: .***5</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Nice product.</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Buyer: r***a</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3496,17 +3496,17 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Tag Heuer 27 Degree 6041 Matte Black / Gray Polyvalent Sunglasses TH6041 101</t>
+          <t>Adidas A644 40 6052 Green Eyeglasses 644 406052 52mm</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>I bought my second pair of these. A happy purchase and service. Thank you.</t>
+          <t>easy buy. great glasses and recieved some nice extras along with them. thank you very much. will purchase again.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Buyer: m***w</t>
+          <t>Buyer: o***g</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3523,17 +3523,17 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Adidas A621 40 6053 Red Eyeglasses 621 406053 50mm</t>
+          <t>MontBlanc Silver / Gray Sunglasses MB457S 16A</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Item exactly as described and shipping was very quick. Thank you!</t>
+          <t>Great product and fast shopping. Thank you! A+++++++</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Buyer: k***k</t>
+          <t>Buyer: .***5</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3555,94 +3555,94 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
+          <t>Nice product.</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Buyer: r***a</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Tag Heuer 27 Degree 6041 Matte Black / Gray Polyvalent Sunglasses TH6041 101</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>I bought my second pair of these. A happy purchase and service. Thank you.</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Buyer: m***w</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Adidas A621 40 6053 Red Eyeglasses 621 406053 50mm</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Item exactly as described and shipping was very quick. Thank you!</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Buyer: k***k</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>More than a year ago</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Positive feedback rating</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
           <t>Top quality!! Very Happy!! Fantastic item! 
 Super quick post! Excellent top seller! Best quality product !!</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr">
+      <c r="D119" t="inlineStr">
         <is>
           <t>Buyer: d***r</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Tom Ford 5415 001 Black Eyeglasses TF5415 001 50mm</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Five star seller.</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Buyer: n***f</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Accurately photographed and described! Great bargain.It is so pretty and soft. It was packaged very nicely and included a personal thank you.</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Buyer: a***0</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>More than a year ago</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>Positive feedback rating</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Bolle Hamilton Shiny Black / True Neutral Smoke TNS Sunglasses 11282</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Just as advertised. Quick shipping and a few freebies.</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Buyer: w***r</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3659,17 +3659,17 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Tag Heuer 823 004 Automatic Blue Gray Eyeglasses TH823-004 52mm</t>
+          <t>Tom Ford 5415 001 Black Eyeglasses TF5415 001 50mm</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Very fast shipping!</t>
+          <t>Five star seller.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Buyer: k***e</t>
+          <t>Buyer: n***f</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -3686,17 +3686,17 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>MONTBLANC MB593 01D Shiny Black / Gray Polarized Sunglasses MB 593 01D</t>
+          <t>GUCCI Shiny Brown Leather Eyeglasses Case Sunglasses Small</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Everything came as expected. A+</t>
+          <t>Accurately photographed and described! Great bargain.It is so pretty and soft. It was packaged very nicely and included a personal thank you.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Buyer: y***n</t>
+          <t>Buyer: a***0</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
+          <t>Bolle Hamilton Shiny Black / True Neutral Smoke TNS Sunglasses 11282</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>A+++ Seller. Gr8 quality product , very reasonably priced &amp; delivery was quick. Thank u.</t>
+          <t>Just as advertised. Quick shipping and a few freebies.</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Buyer: a***4</t>
+          <t>Buyer: w***r</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3740,17 +3740,17 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>ZERORH+ FUXION Matte Black / Grey Polarized Sunglasses RH777-04 CARL ZEISS</t>
+          <t>Tag Heuer 823 004 Automatic Blue Gray Eyeglasses TH823-004 52mm</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>super!!!</t>
+          <t>Very fast shipping!</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Buyer: l***t</t>
+          <t>Buyer: k***e</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3767,17 +3767,17 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Moncler MC507-05 Crystal / Brown Pelvoux Sunglasses MC 507-05</t>
+          <t>MONTBLANC MB593 01D Shiny Black / Gray Polarized Sunglasses MB 593 01D</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Great experience. Great value. Great customer service.</t>
+          <t>Everything came as expected. A+</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Buyer: g***t</t>
+          <t>Buyer: y***n</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -3794,17 +3794,17 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6058 INVOKE Onix / Black Eyeglasses AF20 006058 54mm</t>
+          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Awesome!</t>
+          <t>A+++ Seller. Gr8 quality product , very reasonably priced &amp; delivery was quick. Thank u.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Buyer: ****w</t>
+          <t>Buyer: a***4</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3821,17 +3821,17 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Barton Perreira HEIST Gold Tortoise / Green Sunglasses HEC GOL BTG</t>
+          <t>ZERORH+ FUXION Matte Black / Grey Polarized Sunglasses RH777-04 CARL ZEISS</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Excellent. Very fast shipping. Many thanks.</t>
+          <t>super!!!</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Buyer: l***s</t>
+          <t>Buyer: l***t</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3848,17 +3848,17 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Tom Ford 5590-B 055 Havana Titanium Gold / Blue Block Eyeglasses TF5590 055 50mm</t>
+          <t>Moncler MC507-05 Crystal / Brown Pelvoux Sunglasses MC 507-05</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Ok</t>
+          <t>Great experience. Great value. Great customer service.</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Buyer: 0***e</t>
+          <t>Buyer: g***t</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -3875,17 +3875,17 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Barton Perreira HEIST Gold Tortoise / Green Sunglasses HEC GOL BTG</t>
+          <t>Adidas AF20 00 6058 INVOKE Onix / Black Eyeglasses AF20 006058 54mm</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Excellent. Very fast shipping. Many thanks.</t>
+          <t>Awesome!</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Buyer: l***s</t>
+          <t>Buyer: ****w</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -3902,17 +3902,17 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Adidas A628 40 6053 Chocolate Brown Eyeglasses 628 406053 55mm</t>
+          <t>Barton Perreira HEIST Gold Tortoise / Green Sunglasses HEC GOL BTG</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>as described</t>
+          <t>Excellent. Very fast shipping. Many thanks.</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Buyer: w***_</t>
+          <t>Buyer: l***s</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -3929,17 +3929,17 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>ZERORH+ ZETHA Matte Black / Green Sunglasses RH771-02 ZEISS</t>
+          <t>Tom Ford 5590-B 055 Havana Titanium Gold / Blue Block Eyeglasses TF5590 055 50mm</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>The best seller on the ebay!!!! Thank you!</t>
+          <t>Ok</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Buyer: e***n</t>
+          <t>Buyer: 0***e</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -3956,17 +3956,17 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Adidas AF20 00 6057 INVOKE Amazon Red / Black Eyeglasses AF20 006057 56mm</t>
+          <t>Barton Perreira HEIST Gold Tortoise / Green Sunglasses HEC GOL BTG</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Bin so froh dieses Gestell bekommen zu haben! Dann noch zu einem mega Preis. Die Lieferung war super schnell innerhalb von 11 Tagen. 19 Tage eher als angekündigt. Ich würde bei Sunraycity jederzeit wieder kaufen!</t>
+          <t>Excellent. Very fast shipping. Many thanks.</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Buyer: v***8</t>
+          <t>Buyer: l***s</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -3983,17 +3983,17 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Tom Ford 5694 030 Clear Gold Eyeglasses TF5694 030 54mm</t>
+          <t>Adidas A628 40 6053 Chocolate Brown Eyeglasses 628 406053 55mm</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Quality of the glasses is great! I found this style while visiting my optometry and the price is insane even with insurance. I'm so glad I was able to find a seller who has a reasonable priced stock. Thank you very much!</t>
+          <t>as described</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Buyer: i***n</t>
+          <t>Buyer: w***_</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -4010,17 +4010,17 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Adidas AF13 50 6056 STREAMLIGHT Black Eyeglasses AF13 506056 52mm</t>
+          <t>ZERORH+ ZETHA Matte Black / Green Sunglasses RH771-02 ZEISS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Nice looking item. Fast delivery, thank you</t>
+          <t>The best seller on the ebay!!!! Thank you!</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Buyer: r***a</t>
+          <t>Buyer: e***n</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -4037,17 +4037,17 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Adidas AF22 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF22 406053 54mm</t>
+          <t>Adidas AF20 00 6057 INVOKE Amazon Red / Black Eyeglasses AF20 006057 56mm</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Arrived well in advance. Great vendor. Thank you.</t>
+          <t>Bin so froh dieses Gestell bekommen zu haben! Dann noch zu einem mega Preis. Die Lieferung war super schnell innerhalb von 11 Tagen. 19 Tage eher als angekündigt. Ich würde bei Sunraycity jederzeit wieder kaufen!</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Buyer: j***.</t>
+          <t>Buyer: v***8</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -4064,17 +4064,17 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Tom Ford Colette Gunmetal Black / Gray Gradient Sunglasses TF250 08C</t>
+          <t>Tom Ford 5694 030 Clear Gold Eyeglasses TF5694 030 54mm</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Fast shipping, thanks!</t>
+          <t>Quality of the glasses is great! I found this style while visiting my optometry and the price is insane even with insurance. I'm so glad I was able to find a seller who has a reasonable priced stock. Thank you very much!</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Buyer: 1***e</t>
+          <t>Buyer: i***n</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -4091,17 +4091,17 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Tag Heuer 0552-005 B URBAN Matte Black Red Eyeglasses TH552-005 57mm</t>
+          <t>Adidas AF13 50 6056 STREAMLIGHT Black Eyeglasses AF13 506056 52mm</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Best seller, really recommended</t>
+          <t>Nice looking item. Fast delivery, thank you</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Buyer: g***b</t>
+          <t>Buyer: r***a</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -4118,17 +4118,17 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Tod's 28 5901F Shiny Black / Gradient Brown Sunglasses TO 0028 01F</t>
+          <t>Adidas AF22 40 6053 INVOKE Iron / Dark Gray Eyeglasses AF22 406053 54mm</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Thank you very much for your fast &amp; easy transaction</t>
+          <t>Arrived well in advance. Great vendor. Thank you.</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Buyer: 8***s</t>
+          <t>Buyer: j***.</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -4145,17 +4145,17 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>MONTBLANC MB0732 016  Shiny Palladium Eyeglasses MB 732 016 51mm</t>
+          <t>Tom Ford Colette Gunmetal Black / Gray Gradient Sunglasses TF250 08C</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Very nice product, fast shipping.</t>
+          <t>Fast shipping, thanks!</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Buyer: i***i</t>
+          <t>Buyer: 1***e</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -4172,17 +4172,17 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Adidas AF22 50 6054 INVOKE Black Eyeglasses AF22 506054 54mm</t>
+          <t>Tag Heuer 0552-005 B URBAN Matte Black Red Eyeglasses TH552-005 57mm</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Thank You very much, again, best experience.</t>
+          <t>Best seller, really recommended</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Buyer: s***v</t>
+          <t>Buyer: g***b</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -4199,17 +4199,17 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>St Dupont 721 6052 Silver / Green Sunglasses 65mm</t>
+          <t>Tod's 28 5901F Shiny Black / Gradient Brown Sunglasses TO 0028 01F</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Item exactly as described, came quicker than expected. Thanks for a smooth transaction!</t>
+          <t>Thank you very much for your fast &amp; easy transaction</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Buyer: 2***a</t>
+          <t>Buyer: 8***s</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -4226,17 +4226,17 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Adidas A674 40 6060 Copper Eyeglasses 674 406060 50mm</t>
+          <t>MONTBLANC MB0732 016  Shiny Palladium Eyeglasses MB 732 016 51mm</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>A+ Seller!</t>
+          <t>Very nice product, fast shipping.</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Buyer: d***1</t>
+          <t>Buyer: i***i</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -4253,17 +4253,17 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Tom Ford William 207 09J Gunmetal Gray / Brown Aviator Sunglasses TF207 09J</t>
+          <t>Adidas AF22 50 6054 INVOKE Black Eyeglasses AF22 506054 54mm</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Xactly as promised.</t>
+          <t>Thank You very much, again, best experience.</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Buyer: 1***0</t>
+          <t>Buyer: s***v</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -4280,17 +4280,17 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Tom Ford 5313 098 Green Horn Eyeglasses TF5313 098 55mm</t>
+          <t>St Dupont 721 6052 Silver / Green Sunglasses 65mm</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Incredibly grateful to this seller! Frames were perfect and they were able to expedite the shipping for me so I could get my prescription made in time for a trip. Thank you!</t>
+          <t>Item exactly as described, came quicker than expected. Thanks for a smooth transaction!</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Buyer: b***a</t>
+          <t>Buyer: 2***a</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -4307,17 +4307,17 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>St Dupont 728 6052 Matte Silver / Blue Sunglasses 70mm</t>
+          <t>Adidas A674 40 6060 Copper Eyeglasses 674 406060 50mm</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Got refund quickly after item was returned</t>
+          <t>A+ Seller!</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Buyer: 8***j</t>
+          <t>Buyer: d***1</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -4334,17 +4334,17 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
+          <t>Tom Ford William 207 09J Gunmetal Gray / Brown Aviator Sunglasses TF207 09J</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Exactly what I needed. This was perfect &amp; in excellent condition.</t>
+          <t>Xactly as promised.</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Buyer: l***c</t>
+          <t>Buyer: 1***0</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -4361,17 +4361,17 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Tom Ford Eliott Black Silver / Blue Gradient Sunglasses TF335 02W</t>
+          <t>Tom Ford 5313 098 Green Horn Eyeglasses TF5313 098 55mm</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Nice sunglasses, thank u.</t>
+          <t>Incredibly grateful to this seller! Frames were perfect and they were able to expedite the shipping for me so I could get my prescription made in time for a trip. Thank you!</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Buyer: _***d</t>
+          <t>Buyer: b***a</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -4388,17 +4388,17 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Tag Heuer Ayrton Senna 0253 Matte Black / Green Outdoors Sunglasses TH 253 301</t>
+          <t>St Dupont 728 6052 Matte Silver / Blue Sunglasses 70mm</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Excellent service ! FAST DELIVERY!!  Thanks.</t>
+          <t>Got refund quickly after item was returned</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Buyer: 0***1</t>
+          <t>Buyer: 8***j</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -4415,17 +4415,17 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>MONCLER MC023-V02 White Gold Eyeglasses MC 023-V02</t>
+          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Great transaction. Highly recommended seller</t>
+          <t>Exactly what I needed. This was perfect &amp; in excellent condition.</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Buyer: x***o</t>
+          <t>Buyer: l***c</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -4442,17 +4442,17 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Tom Ford 685 Julie Shiny Black Dark Havana / Brown Sunglasses TF685 05E 52mm</t>
+          <t>Tom Ford Eliott Black Silver / Blue Gradient Sunglasses TF335 02W</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Excellent shopping experience.</t>
+          <t>Nice sunglasses, thank u.</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Buyer: s***s</t>
+          <t>Buyer: _***d</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -4469,17 +4469,17 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>MontBlanc Silver Black / Gray Sunglasses MB458S 16B</t>
+          <t>Tag Heuer Ayrton Senna 0253 Matte Black / Green Outdoors Sunglasses TH 253 301</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Excellent product, though not in original box. But otherwise great.</t>
+          <t>Excellent service ! FAST DELIVERY!!  Thanks.</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Buyer: a***a</t>
+          <t>Buyer: 0***1</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -4496,17 +4496,17 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Tom Ford 5415 054 Tortoise Eyeglasses TF5415 054 50mm</t>
+          <t>MONCLER MC023-V02 White Gold Eyeglasses MC 023-V02</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Excellent frames as described. Thank you!</t>
+          <t>Great transaction. Highly recommended seller</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Buyer: v***v</t>
+          <t>Buyer: x***o</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -4523,17 +4523,17 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Tom Ford Rickie Gold Black / Gray Gradient Sunglasses TF179 01B</t>
+          <t>Tom Ford 685 Julie Shiny Black Dark Havana / Brown Sunglasses TF685 05E 52mm</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Trustworthy seller just as described</t>
+          <t>Excellent shopping experience.</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Buyer: -***z</t>
+          <t>Buyer: s***s</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -4550,17 +4550,17 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>CARRERA VENT-X Gray &amp; Brown / Brown Polarized Sunglasses 6CL PK</t>
+          <t>MontBlanc Silver Black / Gray Sunglasses MB458S 16B</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Good deal thank you</t>
+          <t>Excellent product, though not in original box. But otherwise great.</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Buyer: 3***p</t>
+          <t>Buyer: a***a</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -4577,17 +4577,17 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>JULBO DIRT Black / Gray Sunglasses 369 122</t>
+          <t>Tom Ford 5415 054 Tortoise Eyeglasses TF5415 054 50mm</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Perfect.. thank you!!!</t>
+          <t>Excellent frames as described. Thank you!</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Buyer: a***m</t>
+          <t>Buyer: v***v</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4604,17 +4604,17 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Carrera Carrerino 11 003 Black Yellow / Gray Gradient Sunglasses 55mm</t>
+          <t>Tom Ford Rickie Gold Black / Gray Gradient Sunglasses TF179 01B</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Very Fast, Very Friendly  Safe Seller  A+++++  Thank You !</t>
+          <t>Trustworthy seller just as described</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Buyer: e***e</t>
+          <t>Buyer: -***z</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4631,17 +4631,17 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Tom Ford NIKA Shiny Black / Blue Gradient Sunglasses TF523 01W</t>
+          <t>CARRERA VENT-X Gray &amp; Brown / Brown Polarized Sunglasses 6CL PK</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Quick Shipping and just as described!</t>
+          <t>Good deal thank you</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Buyer: d***i</t>
+          <t>Buyer: 3***p</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -4658,17 +4658,17 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>MontBlanc Gold / Polarized Brown Sunglasses MB703S 32H 703 61mm</t>
+          <t>JULBO DIRT Black / Gray Sunglasses 369 122</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Moshe of Sunraycity provides excellent service from my initial question to the  dispatching of goods. The item has arrived package with surprise gift and a personal care card. Definitely a business worth supporting.</t>
+          <t>Perfect.. thank you!!!</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Buyer: t***m</t>
+          <t>Buyer: a***m</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -4685,17 +4685,17 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Serengeti Trapani Shiny Silver Smoke / 555nm Sunglasses 7603 60mm</t>
+          <t>Carrera Carrerino 11 003 Black Yellow / Gray Gradient Sunglasses 55mm</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Your package that you sent arrived on time</t>
+          <t>Very Fast, Very Friendly  Safe Seller  A+++++  Thank You !</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Buyer: t***v</t>
+          <t>Buyer: e***e</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -4712,17 +4712,17 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Tag Heuer 3052 001 Reflex Black Eyeglasses TH3052-001 47mm</t>
+          <t>Tom Ford NIKA Shiny Black / Blue Gradient Sunglasses TF523 01W</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>perfect</t>
+          <t>Quick Shipping and just as described!</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Buyer: l***p</t>
+          <t>Buyer: d***i</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -4739,17 +4739,17 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Bolle Stormy Shiny Black TNS Sunglasses 11177</t>
+          <t>MontBlanc Gold / Polarized Brown Sunglasses MB703S 32H 703 61mm</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Authentic product. Fast shipping and great transaction. Thank you!</t>
+          <t>Moshe of Sunraycity provides excellent service from my initial question to the  dispatching of goods. The item has arrived package with surprise gift and a personal care card. Definitely a business worth supporting.</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Buyer: 6***i</t>
+          <t>Buyer: t***m</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -4766,17 +4766,17 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Barton Perreira GINSBERG Gold Eyeglasses GOL 46mm</t>
+          <t>Serengeti Trapani Shiny Silver Smoke / 555nm Sunglasses 7603 60mm</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Great eyeglasses + excellent transaction. Thank you!</t>
+          <t>Your package that you sent arrived on time</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Buyer: 2***e</t>
+          <t>Buyer: t***v</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -4793,17 +4793,17 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Serengeti Assisi Matte Brown / Polarized Phd Drivers Sunglasses 7996</t>
+          <t>Tag Heuer 3052 001 Reflex Black Eyeglasses TH3052-001 47mm</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Fast delivery, good communication</t>
+          <t>perfect</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Buyer: o***s</t>
+          <t>Buyer: l***p</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -4820,17 +4820,17 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Tom Ford 5430 052 Dark Havana Eyeglasses TF5430 052 56mm</t>
+          <t>Bolle Stormy Shiny Black TNS Sunglasses 11177</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Very easy deal and fast delivery. Thanks!</t>
+          <t>Authentic product. Fast shipping and great transaction. Thank you!</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Buyer: p***r</t>
+          <t>Buyer: 6***i</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -4847,17 +4847,17 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Tom Ford 5272-005 Black Gold Eyeglasses TF5272 005 53mm</t>
+          <t>Barton Perreira GINSBERG Gold Eyeglasses GOL 46mm</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Great service!</t>
+          <t>Great eyeglasses + excellent transaction. Thank you!</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Buyer: r***1</t>
+          <t>Buyer: 2***e</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -4874,17 +4874,17 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Serengeti TREVISO 24h LEMANS Satin Gunmetal / Green Polarized Sunglasses 8483</t>
+          <t>Serengeti Assisi Matte Brown / Polarized Phd Drivers Sunglasses 7996</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>Fast delivery, good communication</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Buyer: 6***0</t>
+          <t>Buyer: o***s</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -4901,17 +4901,17 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Tag Heuer 842 008 Automatic Matte Blue Gray Eyeglasses TH842-008 54mm</t>
+          <t>Tom Ford 5430 052 Dark Havana Eyeglasses TF5430 052 56mm</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Great dealer, A++++++++++++ product, fast shipping</t>
+          <t>Very easy deal and fast delivery. Thanks!</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Buyer: l***e</t>
+          <t>Buyer: p***r</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -4928,17 +4928,17 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Serengeti Martino Shiny Black / Polarized Drivers Sunglasses 7489 60mm</t>
+          <t>Tom Ford 5272-005 Black Gold Eyeglasses TF5272 005 53mm</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Producto en excelente estado</t>
+          <t>Great service!</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Buyer: 9***g</t>
+          <t>Buyer: r***1</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -4955,17 +4955,17 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Tom Ford 5628 005 Asian Fit Shiny Black / Blue Block Eyeglasses TF5628 005 54mm</t>
+          <t>Serengeti TREVISO 24h LEMANS Satin Gunmetal / Green Polarized Sunglasses 8483</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Thanks!</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Buyer: m***m</t>
+          <t>Buyer: 6***0</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -4982,17 +4982,17 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Spy Hailwood Shiny Black / Gray Sunglasses</t>
+          <t>Tag Heuer 842 008 Automatic Matte Blue Gray Eyeglasses TH842-008 54mm</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Fast shipping!!! Great sunglasses!!!!</t>
+          <t>Great dealer, A++++++++++++ product, fast shipping</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Buyer: 0***r</t>
+          <t>Buyer: l***e</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -5009,17 +5009,17 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Tom Ford 5353 001 Shiny Black Gold Eyeglasses TF5353 001 52mm</t>
+          <t>Serengeti Martino Shiny Black / Polarized Drivers Sunglasses 7489 60mm</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Amazing seller, well packaged, speedy shipping, highly recommended A++++++++++++++</t>
+          <t>Producto en excelente estado</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Buyer: s***s</t>
+          <t>Buyer: 9***g</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -5036,17 +5036,17 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Tom Ford Magnus Gold / Brown Sunglasses TF193 28E</t>
+          <t>Tom Ford 5628 005 Asian Fit Shiny Black / Blue Block Eyeglasses TF5628 005 54mm</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Excellent seller and exceptional team.  Smooth transaction and highly recommended.</t>
+          <t>Thanks!</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Buyer: l***s</t>
+          <t>Buyer: m***m</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -5063,17 +5063,17 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Tag Heuer 3052 001 Reflex Black Eyeglasses TH3052-001 47mm</t>
+          <t>Spy Hailwood Shiny Black / Gray Sunglasses</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Best seller ever, amazing communication, highly recommended</t>
+          <t>Fast shipping!!! Great sunglasses!!!!</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Buyer: _***l</t>
+          <t>Buyer: 0***r</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -5090,17 +5090,17 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Serengeti Luigi Gun Black Tannery / Polarized Green Sunglasses 7382</t>
+          <t>Tom Ford 5353 001 Shiny Black Gold Eyeglasses TF5353 001 52mm</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>pleased to deal with you. I'm definitely a fan of Serengeti. Perfect pair of sunglasses.</t>
+          <t>Amazing seller, well packaged, speedy shipping, highly recommended A++++++++++++++</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Buyer: v***l</t>
+          <t>Buyer: s***s</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -5117,17 +5117,17 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Adidas A3 40 6051 Copper Brown Eyeglasses A003 40 6051 50mm</t>
+          <t>Tom Ford Magnus Gold / Brown Sunglasses TF193 28E</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Got it plus some nice bonus items with my glasses frames.</t>
+          <t>Excellent seller and exceptional team.  Smooth transaction and highly recommended.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Buyer: p***7</t>
+          <t>Buyer: l***s</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -5144,17 +5144,17 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Tom Ford 5527 066 Red Eyeglasses TF5527 066 50mm</t>
+          <t>Tag Heuer 3052 001 Reflex Black Eyeglasses TH3052-001 47mm</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>GREAT TRANSACTION!!</t>
+          <t>Best seller ever, amazing communication, highly recommended</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Buyer: l***6</t>
+          <t>Buyer: _***l</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -5171,17 +5171,17 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Barton Perreira REECE Black / Vintage Blue Sunglasses BLA VBL 52mm</t>
+          <t>Serengeti Luigi Gun Black Tannery / Polarized Green Sunglasses 7382</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Perfect Seller and Transaction.  5*****</t>
+          <t>pleased to deal with you. I'm definitely a fan of Serengeti. Perfect pair of sunglasses.</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Buyer: 0***0</t>
+          <t>Buyer: v***l</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -5198,17 +5198,17 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Serengeti Strato Satin Black / Polarized Phd Sedona Sunglasses 7681</t>
+          <t>Adidas A3 40 6051 Copper Brown Eyeglasses A003 40 6051 50mm</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Just what I ordered. Thank you.</t>
+          <t>Got it plus some nice bonus items with my glasses frames.</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Buyer: r***c</t>
+          <t>Buyer: p***7</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -5225,17 +5225,17 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Tom Ford Snowdon Beige / Gray Gradient Sunglasses TF237 60B 50mm</t>
+          <t>Tom Ford 5527 066 Red Eyeglasses TF5527 066 50mm</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Lightning fast shipping and great transaction.</t>
+          <t>GREAT TRANSACTION!!</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Buyer: i***i</t>
+          <t>Buyer: l***6</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -5252,17 +5252,17 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
+          <t>Barton Perreira REECE Black / Vintage Blue Sunglasses BLA VBL 52mm</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Great transaction, thank you</t>
+          <t>Perfect Seller and Transaction.  5*****</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Buyer: j***j</t>
+          <t>Buyer: 0***0</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -5279,17 +5279,17 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Tom Ford Snowdon Dark Havana / Green Sunglasses TF237 52N 50mm</t>
+          <t>Serengeti Strato Satin Black / Polarized Phd Sedona Sunglasses 7681</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>EXCELLENT FAST SELLER !!  ITEM EXACTLY AS DESCRIBED.  FULLY LEGIT ...</t>
+          <t>Just what I ordered. Thank you.</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Buyer: .***.</t>
+          <t>Buyer: r***c</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -5306,17 +5306,17 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Serengeti NUVINO Shiny Black / Polarized Phd Cool Photo Gray CPG Sunglasses 7318</t>
+          <t>Tom Ford Snowdon Beige / Gray Gradient Sunglasses TF237 60B 50mm</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Thanks item as described and shipped fast.  Thanks.</t>
+          <t>Lightning fast shipping and great transaction.</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Buyer: h***e</t>
+          <t>Buyer: i***i</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -5333,17 +5333,17 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Serengeti Larino Carbon Fiber / Polarized Phd CPG Sunglasses 7710</t>
+          <t>Bolle FLYAIR Matte Tortoise / True Light Brown TLB Sunglasses 12260</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Thank You!!</t>
+          <t>Great transaction, thank you</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Buyer: o***3</t>
+          <t>Buyer: j***j</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -5360,17 +5360,17 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Tom Ford Nicholai Gold / Brown Sunglasses TF189 28J James Bond</t>
+          <t>Tom Ford Snowdon Dark Havana / Green Sunglasses TF237 52N 50mm</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Very happy and arrived within a few weeks</t>
+          <t>EXCELLENT FAST SELLER !!  ITEM EXACTLY AS DESCRIBED.  FULLY LEGIT ...</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Buyer: u***s</t>
+          <t>Buyer: .***.</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -5387,17 +5387,17 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Tom Ford 5475 32E Gold Eyeglasses TF5475-32E with Magnetic Brown Clip 54mm</t>
+          <t>Serengeti NUVINO Shiny Black / Polarized Phd Cool Photo Gray CPG Sunglasses 7318</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Fantastic, love these Glasses… very good company and will certainly purchase from them again</t>
+          <t>Thanks item as described and shipped fast.  Thanks.</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Buyer: b***a</t>
+          <t>Buyer: h***e</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -5414,17 +5414,17 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
+          <t>Serengeti Larino Carbon Fiber / Polarized Phd CPG Sunglasses 7710</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Great seller...item exactly as presented.. thank you</t>
+          <t>Thank You!!</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Buyer: a***p</t>
+          <t>Buyer: o***3</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -5441,17 +5441,17 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Tom Ford 5420 074 Matte Pink Rose Eyeglasses TF5420 074 54mm</t>
+          <t>Tom Ford Nicholai Gold / Brown Sunglasses TF189 28J James Bond</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Beautiful frames!</t>
+          <t>Very happy and arrived within a few weeks</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Buyer: d***a</t>
+          <t>Buyer: 6***r</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -5468,17 +5468,17 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Bolle Vortex Shiny Black / Gray PC True Neutral Smoke TNS Sunglasses 11858</t>
+          <t>Tom Ford 5475 32E Gold Eyeglasses TF5475-32E with Magnetic Brown Clip 54mm</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Great sunglasses thanks !!!</t>
+          <t>Fantastic, love these Glasses… very good company and will certainly purchase from them again</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Buyer: l***e</t>
+          <t>Buyer: b***a</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -5495,17 +5495,17 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Tom Ford 5527 052 Havana Eyeglasses TF5527 052 50mm</t>
+          <t>GUCCI GOLD BROWN LARGE CLAMSHELL LEATHER CASE WITH CLOTH &amp; CARDBOARD BOX</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Good product</t>
+          <t>Great seller...item exactly as presented.. thank you</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Buyer: c***a</t>
+          <t>Buyer: a***p</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -5522,17 +5522,17 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Tom Ford Snowdon Dark Havana / Green Sunglasses TF237 52N 50mm</t>
+          <t>Tom Ford 5420 074 Matte Pink Rose Eyeglasses TF5420 074 54mm</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Great product</t>
+          <t>Beautiful frames!</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Buyer: c***a</t>
+          <t>Buyer: d***a</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -5549,17 +5549,17 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Tom Ford 5586-B 052 Havana Blue Block Eyeglasses TF5586 052 56mm</t>
+          <t>Bolle Vortex Shiny Black / Gray PC True Neutral Smoke TNS Sunglasses 11858</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Everything was as expected and communicated. Very happy!</t>
+          <t>Great sunglasses thanks !!!</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Buyer: m***a</t>
+          <t>Buyer: l***e</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -5576,17 +5576,17 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Tom Ford BRADBURY Shiny Rose Gold / Gray Sunglasses TF525 28A</t>
+          <t>Tom Ford 5527 052 Havana Eyeglasses TF5527 052 50mm</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Great seller, great quality, received cleaning agent as well and item came way before time.</t>
+          <t>Good product</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Buyer: p***0</t>
+          <t>Buyer: c***a</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -5603,17 +5603,17 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Barton Perreira GINSBERG Matte Black Eyeglasses MAB 46mm</t>
+          <t>Tom Ford Snowdon Dark Havana / Green Sunglasses TF237 52N 50mm</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>++++++++++++++ as advertised +++++++++++++</t>
+          <t>Great product</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Buyer: u***l</t>
+          <t>Buyer: c***a</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -5630,17 +5630,17 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Serengeti Verucchio Shiny Black / Polarized Phd CPG Sunglasses 7440</t>
+          <t>Tom Ford 5586-B 052 Havana Blue Block Eyeglasses TF5586 052 56mm</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>I got it. thanks.</t>
+          <t>Everything was as expected and communicated. Very happy!</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Buyer: l***a</t>
+          <t>Buyer: m***a</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -5657,17 +5657,17 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Tom Ford 5346 052 Dark Havana Eyeglasses TF5346 052 53mm</t>
+          <t>Tom Ford BRADBURY Shiny Rose Gold / Gray Sunglasses TF525 28A</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Speedy shipping, careful packaging, will do business again!</t>
+          <t>Great seller, great quality, received cleaning agent as well and item came way before time.</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Buyer: h***a</t>
+          <t>Buyer: p***0</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -5684,17 +5684,17 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Spy Logan Shiny Black / Gray Sunglasses</t>
+          <t>Barton Perreira GINSBERG Matte Black Eyeglasses MAB 46mm</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>wonderful seller,  I highly recommend others to this seller, wonderful communication and service,  I'm very happy with my purchase,  thank you. It fits perfect, will definitely buy another.</t>
+          <t>++++++++++++++ as advertised +++++++++++++</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Buyer: d***d</t>
+          <t>Buyer: u***l</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -5711,17 +5711,17 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Persol 3097S 101857 Light Brown / Brown Polarized Sunglasses PO3097</t>
+          <t>Serengeti Verucchio Shiny Black / Polarized Phd CPG Sunglasses 7440</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>They included a free mask!</t>
+          <t>I got it. thanks.</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Buyer: m***k</t>
+          <t>Buyer: l***a</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -5738,17 +5738,17 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Serengeti Dante Shiny Silver / 555nm Green Sunglasses 7314</t>
+          <t>Tom Ford 5346 052 Dark Havana Eyeglasses TF5346 052 53mm</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Very fast shipping with great communication!!</t>
+          <t>Speedy shipping, careful packaging, will do business again!</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Buyer: v***v</t>
+          <t>Buyer: h***a</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -5765,17 +5765,17 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>MONCLER MC019-V01 Gray Eyeglasses MC 019-V01</t>
+          <t>Spy Logan Shiny Black / Gray Sunglasses</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Very happy with item, thank you.</t>
+          <t>wonderful seller,  I highly recommend others to this seller, wonderful communication and service,  I'm very happy with my purchase,  thank you. It fits perfect, will definitely buy another.</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Buyer: t***i</t>
+          <t>Buyer: d***d</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -5792,17 +5792,17 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Tom Ford ARNAUD 625 52V Havana Gold / Blue Sunglasses TF625 52V 53mm</t>
+          <t>Persol 3097S 101857 Light Brown / Brown Polarized Sunglasses PO3097</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>AAA+++ Great seller!</t>
+          <t>They included a free mask!</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Buyer: d***d</t>
+          <t>Buyer: m***k</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -5819,17 +5819,17 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Tom Ford Marko Gunmetal / Gray Sunglasses TF144 08B</t>
+          <t>Serengeti Dante Shiny Silver / 555nm Green Sunglasses 7314</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>very happy with the purchase and experience.</t>
+          <t>Very fast shipping with great communication!!</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Buyer: 2***r</t>
+          <t>Buyer: v***v</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -5846,17 +5846,17 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Tom Ford NIKA Black Ivory / Gray Gradient Sunglasses TF523 01B</t>
+          <t>MONCLER MC019-V01 Gray Eyeglasses MC 019-V01</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Beautiful item</t>
+          <t>Very happy with item, thank you.</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Buyer: w***0</t>
+          <t>Buyer: t***i</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">

</xml_diff>